<commit_message>
Completed Gateway Comparison Matrix
</commit_message>
<xml_diff>
--- a/Sem2-Assignments-Gantt-Chart.xlsx
+++ b/Sem2-Assignments-Gantt-Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\TAFE\Dual-Diploma-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA89925-3BD0-40DC-B01F-65F26621C1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87010641-8D4B-42FF-A355-9FDE823283F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A21A907-22B3-4C37-9935-FF093452207E}"/>
   </bookViews>
@@ -1577,7 +1577,7 @@
       <pane xSplit="9" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Due dates to include Web App Dev classes
</commit_message>
<xml_diff>
--- a/Sem2-Assignments-Gantt-Chart.xlsx
+++ b/Sem2-Assignments-Gantt-Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\TAFE\Dual-Diploma-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34B9920-9E56-481E-9D88-C39F33063787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A231E23E-915D-478D-B42A-0AC9D793462A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A21A907-22B3-4C37-9935-FF093452207E}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="105">
   <si>
     <t>Activity</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>Overdue</t>
-  </si>
-  <si>
-    <t>NO LAP</t>
   </si>
   <si>
     <t>AT2 (A) – Documentation (Part 1)</t>
@@ -396,22 +393,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Web App Development </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(NO LAP)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>SaaS</t>
     </r>
     <r>
@@ -592,6 +573,21 @@
   <si>
     <t>Update Info Architecture LAP Due Dates'</t>
   </si>
+  <si>
+    <t>Modularisation Formative Assessment</t>
+  </si>
+  <si>
+    <t>Assessment2 (Build Webpage[components])</t>
+  </si>
+  <si>
+    <t>Assessment3 (BuildWebpage[framework])</t>
+  </si>
+  <si>
+    <t>Web App Development (NO LAP)</t>
+  </si>
+  <si>
+    <t>Web App Development</t>
+  </si>
 </sst>
 </file>
 
@@ -707,7 +703,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -825,6 +821,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1067,7 +1069,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1185,6 +1186,7 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1721,18 +1723,18 @@
   <dimension ref="B1:AK93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="4" topLeftCell="K66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
@@ -1744,62 +1746,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J1" s="67">
+      <c r="J1" s="66">
         <f ca="1">L3</f>
-        <v>45488</v>
-      </c>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="66">
+        <v>45516</v>
+      </c>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="65">
         <f ca="1">Q3</f>
-        <v>45523</v>
-      </c>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66"/>
-      <c r="S1" s="67">
+        <v>45551</v>
+      </c>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="66">
         <f ca="1">U3</f>
-        <v>45551</v>
-      </c>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="66">
+        <v>45579</v>
+      </c>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="65">
         <f ca="1">Z3</f>
-        <v>45586</v>
-      </c>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="67">
+        <v>45614</v>
+      </c>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="66">
         <f ca="1">AD3</f>
-        <v>45614</v>
-      </c>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="66">
+        <v>45642</v>
+      </c>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="65">
         <f ca="1">AH3</f>
-        <v>45642</v>
-      </c>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="66"/>
+        <v>45670</v>
+      </c>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
       <c r="AJ1" s="2"/>
     </row>
     <row r="2" spans="2:37" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="23"/>
-      <c r="C2" s="43">
+      <c r="B2" s="22"/>
+      <c r="C2" s="42">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="23"/>
+        <v>45511</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="22"/>
       <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
@@ -1881,132 +1883,132 @@
       </c>
     </row>
     <row r="3" spans="2:37" ht="39" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="23"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="1"/>
       <c r="I3" s="4"/>
       <c r="K3" s="14">
         <f ca="1">IF(MONTH(C2-WEEKDAY((C2),2)+1)&lt;MONTH(C2),(C2-28-DAY(C2)+7)-WEEKDAY((C2-DAY(C2)+7),2)+1,(C2-DAY(C2)+7)-WEEKDAY((C2-DAY(C2)+7),2)+1)</f>
-        <v>45481</v>
+        <v>45509</v>
       </c>
       <c r="L3" s="14">
         <f ca="1">K3+7</f>
-        <v>45488</v>
+        <v>45516</v>
       </c>
       <c r="M3" s="3">
         <f t="shared" ref="M3:AJ3" ca="1" si="0">L3+7</f>
-        <v>45495</v>
+        <v>45523</v>
       </c>
       <c r="N3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45502</v>
+        <v>45530</v>
       </c>
       <c r="O3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45509</v>
+        <v>45537</v>
       </c>
       <c r="P3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45516</v>
+        <v>45544</v>
       </c>
       <c r="Q3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45523</v>
+        <v>45551</v>
       </c>
       <c r="R3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45530</v>
+        <v>45558</v>
       </c>
       <c r="S3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45537</v>
+        <v>45565</v>
       </c>
       <c r="T3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45544</v>
+        <v>45572</v>
       </c>
       <c r="U3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45551</v>
+        <v>45579</v>
       </c>
       <c r="V3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45558</v>
+        <v>45586</v>
       </c>
       <c r="W3" s="14">
         <f t="shared" ca="1" si="0"/>
-        <v>45565</v>
+        <v>45593</v>
       </c>
       <c r="X3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45572</v>
+        <v>45600</v>
       </c>
       <c r="Y3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45579</v>
+        <v>45607</v>
       </c>
       <c r="Z3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45586</v>
+        <v>45614</v>
       </c>
       <c r="AA3" s="3">
         <f ca="1">Z3+7</f>
-        <v>45593</v>
+        <v>45621</v>
       </c>
       <c r="AB3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45600</v>
+        <v>45628</v>
       </c>
       <c r="AC3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45607</v>
+        <v>45635</v>
       </c>
       <c r="AD3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45614</v>
+        <v>45642</v>
       </c>
       <c r="AE3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45621</v>
+        <v>45649</v>
       </c>
       <c r="AF3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45628</v>
+        <v>45656</v>
       </c>
       <c r="AG3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45635</v>
+        <v>45663</v>
       </c>
       <c r="AH3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45642</v>
+        <v>45670</v>
       </c>
       <c r="AI3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45649</v>
+        <v>45677</v>
       </c>
       <c r="AJ3" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45656</v>
+        <v>45684</v>
       </c>
       <c r="AK3" s="3">
         <f ca="1">AJ3+7</f>
-        <v>45663</v>
+        <v>45691</v>
       </c>
     </row>
     <row r="4" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="16" t="s">
@@ -2018,7 +2020,7 @@
       <c r="G4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="26" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="7"/>
@@ -2052,7 +2054,7 @@
     </row>
     <row r="5" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="19">
         <v>45509</v>
@@ -2060,14 +2062,14 @@
       <c r="D5" s="19">
         <v>45537</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <f t="shared" ref="E5:E36" si="1">IF(D5="","",NETWORKDAYS(C5,D5))</f>
         <v>21</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="23">
         <v>0.05</v>
       </c>
       <c r="H5" s="15" t="s">
@@ -2091,7 +2093,7 @@
       </c>
       <c r="N5" s="18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="O5" s="18" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -2107,7 +2109,7 @@
       </c>
       <c r="R5" s="18" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="S5" s="18" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -2184,7 +2186,7 @@
     </row>
     <row r="6" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="19">
         <v>45544</v>
@@ -2192,14 +2194,14 @@
       <c r="D6" s="19">
         <v>45572</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="23">
         <v>0.05</v>
       </c>
       <c r="H6" s="15" t="s">
@@ -2243,7 +2245,7 @@
       </c>
       <c r="S6" s="18" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="T6" s="18" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2259,7 +2261,7 @@
       </c>
       <c r="W6" s="18" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="X6" s="18" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -2316,7 +2318,7 @@
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="19">
         <v>45488</v>
@@ -2324,14 +2326,14 @@
       <c r="D7" s="19">
         <v>45614</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="23">
         <v>0.05</v>
       </c>
       <c r="H7" s="15" t="s">
@@ -2399,7 +2401,7 @@
       </c>
       <c r="Y7" s="18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Z7" s="18" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2415,7 +2417,7 @@
       </c>
       <c r="AC7" s="18" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AD7" s="18" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -2448,7 +2450,7 @@
     </row>
     <row r="8" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="19">
         <v>45607</v>
@@ -2456,14 +2458,14 @@
       <c r="D8" s="19">
         <v>45618</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="23">
         <v>0.05</v>
       </c>
       <c r="H8" s="15" t="s">
@@ -2531,7 +2533,7 @@
       </c>
       <c r="Y8" s="18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Z8" s="18" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -2547,7 +2549,7 @@
       </c>
       <c r="AC8" s="18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AD8" s="18" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -2580,7 +2582,7 @@
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="19">
         <v>45516</v>
@@ -2588,14 +2590,14 @@
       <c r="D9" s="19">
         <v>45523</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="23">
         <v>0.05</v>
       </c>
       <c r="H9" s="15" t="s">
@@ -2611,7 +2613,7 @@
       </c>
       <c r="L9" s="18" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="M9" s="18" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -2627,7 +2629,7 @@
       </c>
       <c r="P9" s="18" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="Q9" s="18" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -2720,14 +2722,14 @@
       <c r="D10" s="19">
         <v>45537</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="23">
         <v>0.05</v>
       </c>
       <c r="H10" s="15" t="s">
@@ -2751,7 +2753,7 @@
       </c>
       <c r="N10" s="18" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="O10" s="18" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2767,7 +2769,7 @@
       </c>
       <c r="R10" s="18" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="S10" s="18" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -2852,14 +2854,14 @@
       <c r="D11" s="19">
         <v>45537</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="24">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="23">
         <v>0.05</v>
       </c>
       <c r="H11" s="15" t="s">
@@ -2883,7 +2885,7 @@
       </c>
       <c r="N11" s="18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="O11" s="18" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -2899,7 +2901,7 @@
       </c>
       <c r="R11" s="18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="S11" s="18" t="str">
         <f t="shared" ca="1" si="8"/>
@@ -2984,14 +2986,14 @@
       <c r="D12" s="19">
         <v>45537</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="24">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="23">
         <v>0.05</v>
       </c>
       <c r="H12" s="15" t="s">
@@ -3015,7 +3017,7 @@
       </c>
       <c r="N12" s="18" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="O12" s="18" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -3031,7 +3033,7 @@
       </c>
       <c r="R12" s="18" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="S12" s="18" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -3116,14 +3118,14 @@
       <c r="D13" s="19">
         <v>45537</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="24">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="23">
         <v>0.05</v>
       </c>
       <c r="H13" s="15" t="s">
@@ -3147,7 +3149,7 @@
       </c>
       <c r="N13" s="18" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="O13" s="18" t="str">
         <f t="shared" ca="1" si="10"/>
@@ -3163,7 +3165,7 @@
       </c>
       <c r="R13" s="18" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="S13" s="18" t="str">
         <f t="shared" ca="1" si="10"/>
@@ -3240,7 +3242,7 @@
     </row>
     <row r="14" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C14" s="19">
         <v>45523</v>
@@ -3248,14 +3250,14 @@
       <c r="D14" s="19">
         <v>45544</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="24">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="23">
         <v>0.05</v>
       </c>
       <c r="H14" s="15" t="s">
@@ -3283,7 +3285,7 @@
       </c>
       <c r="O14" s="18" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="P14" s="18" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -3299,7 +3301,7 @@
       </c>
       <c r="S14" s="18" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="T14" s="18" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -3372,7 +3374,7 @@
     </row>
     <row r="15" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="19">
         <v>45488</v>
@@ -3380,14 +3382,14 @@
       <c r="D15" s="19">
         <v>45516</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="24">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="23">
         <v>0.05</v>
       </c>
       <c r="H15" s="15" t="s">
@@ -3399,7 +3401,7 @@
       </c>
       <c r="K15" s="17" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="L15" s="18" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -3415,7 +3417,7 @@
       </c>
       <c r="O15" s="18" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="P15" s="18" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -3504,7 +3506,7 @@
     </row>
     <row r="16" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C16" s="19">
         <v>45502</v>
@@ -3512,14 +3514,14 @@
       <c r="D16" s="19">
         <v>45516</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="24">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="23">
         <v>0.05</v>
       </c>
       <c r="H16" s="15" t="s">
@@ -3531,7 +3533,7 @@
       </c>
       <c r="K16" s="17" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="L16" s="18" t="str">
         <f t="shared" ca="1" si="13"/>
@@ -3547,7 +3549,7 @@
       </c>
       <c r="O16" s="18" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="P16" s="18" t="str">
         <f t="shared" ca="1" si="13"/>
@@ -3636,7 +3638,7 @@
     </row>
     <row r="17" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C17" s="19">
         <v>45537</v>
@@ -3644,14 +3646,14 @@
       <c r="D17" s="19">
         <v>45551</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="24">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="23">
         <v>0.05</v>
       </c>
       <c r="H17" s="15" t="s">
@@ -3683,7 +3685,7 @@
       </c>
       <c r="P17" s="18" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Q17" s="18" t="str">
         <f t="shared" ca="1" si="14"/>
@@ -3699,7 +3701,7 @@
       </c>
       <c r="T17" s="18" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="U17" s="18" t="str">
         <f t="shared" ca="1" si="14"/>
@@ -3768,7 +3770,7 @@
     </row>
     <row r="18" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="19">
         <v>45555</v>
@@ -3776,14 +3778,14 @@
       <c r="D18" s="19">
         <v>45593</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="24">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="23">
         <v>0.05</v>
       </c>
       <c r="H18" s="15" t="s">
@@ -3839,7 +3841,7 @@
       </c>
       <c r="V18" s="17" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="W18" s="18" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -3855,7 +3857,7 @@
       </c>
       <c r="Z18" s="18" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AA18" s="18" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -3900,7 +3902,7 @@
     </row>
     <row r="19" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="19">
         <v>45579</v>
@@ -3908,14 +3910,14 @@
       <c r="D19" s="19">
         <v>45593</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="24">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="23">
         <v>0.05</v>
       </c>
       <c r="H19" s="15" t="s">
@@ -3971,7 +3973,7 @@
       </c>
       <c r="V19" s="17" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="W19" s="18" t="str">
         <f t="shared" ca="1" si="16"/>
@@ -3987,7 +3989,7 @@
       </c>
       <c r="Z19" s="18" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AA19" s="18" t="str">
         <f t="shared" ca="1" si="16"/>
@@ -4032,7 +4034,7 @@
     </row>
     <row r="20" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="19">
         <v>45586</v>
@@ -4040,14 +4042,14 @@
       <c r="D20" s="19">
         <v>45593</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="24">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="24">
+      <c r="G20" s="23">
         <v>0.05</v>
       </c>
       <c r="H20" s="15" t="s">
@@ -4103,7 +4105,7 @@
       </c>
       <c r="V20" s="17" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="W20" s="18" t="str">
         <f t="shared" ca="1" si="17"/>
@@ -4119,7 +4121,7 @@
       </c>
       <c r="Z20" s="18" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AA20" s="18" t="str">
         <f t="shared" ca="1" si="17"/>
@@ -4164,7 +4166,7 @@
     </row>
     <row r="21" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="19">
         <v>45600</v>
@@ -4172,14 +4174,14 @@
       <c r="D21" s="19">
         <v>45614</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="24">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="24">
+      <c r="G21" s="23">
         <v>0.05</v>
       </c>
       <c r="H21" s="15" t="s">
@@ -4247,7 +4249,7 @@
       </c>
       <c r="Y21" s="18" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Z21" s="18" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -4263,7 +4265,7 @@
       </c>
       <c r="AC21" s="18" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AD21" s="18" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -4296,7 +4298,7 @@
     </row>
     <row r="22" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="19">
         <v>45600</v>
@@ -4304,14 +4306,14 @@
       <c r="D22" s="19">
         <v>45614</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="24">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="23">
         <v>0.05</v>
       </c>
       <c r="H22" s="15" t="s">
@@ -4379,7 +4381,7 @@
       </c>
       <c r="Y22" s="18" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Z22" s="18" t="str">
         <f t="shared" ca="1" si="19"/>
@@ -4395,7 +4397,7 @@
       </c>
       <c r="AC22" s="18" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AD22" s="18" t="str">
         <f t="shared" ca="1" si="19"/>
@@ -4428,7 +4430,7 @@
     </row>
     <row r="23" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" s="19">
         <v>45600</v>
@@ -4436,14 +4438,14 @@
       <c r="D23" s="19">
         <v>45614</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="24">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="23">
         <v>0.05</v>
       </c>
       <c r="H23" s="15" t="s">
@@ -4505,7 +4507,7 @@
       </c>
       <c r="Y23" s="18" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Z23" s="18" t="str">
         <f t="shared" ca="1" si="20"/>
@@ -4521,7 +4523,7 @@
       </c>
       <c r="AC23" s="18" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AD23" s="18" t="str">
         <f t="shared" ca="1" si="20"/>
@@ -4562,14 +4564,14 @@
       <c r="D24" s="19">
         <v>45509</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="24">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G24" s="24">
+      <c r="G24" s="23">
         <v>0.05</v>
       </c>
       <c r="H24" s="15" t="s">
@@ -4587,7 +4589,7 @@
       </c>
       <c r="N24" s="18" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="O24" s="18" t="str">
         <f t="shared" ca="1" si="21"/>
@@ -4688,14 +4690,14 @@
       <c r="D25" s="19">
         <v>45509</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="24">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="24">
+      <c r="G25" s="23">
         <v>0.05</v>
       </c>
       <c r="H25" s="15" t="s">
@@ -4713,7 +4715,7 @@
       </c>
       <c r="N25" s="18" t="str">
         <f t="shared" ca="1" si="22"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="O25" s="18" t="str">
         <f t="shared" ca="1" si="22"/>
@@ -4814,14 +4816,14 @@
       <c r="D26" s="19">
         <v>45523</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="24">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="23">
         <v>0.05</v>
       </c>
       <c r="H26" s="15" t="s">
@@ -4831,7 +4833,7 @@
       <c r="K26" s="17"/>
       <c r="L26" s="18" t="str">
         <f t="shared" ref="L26:AJ26" ca="1" si="23">IF(M$3=($D26-WEEKDAY($D26,2)+1),"u","")</f>
-        <v/>
+        <v>u</v>
       </c>
       <c r="M26" s="18" t="str">
         <f t="shared" ca="1" si="23"/>
@@ -4847,7 +4849,7 @@
       </c>
       <c r="P26" s="18" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="Q26" s="18" t="str">
         <f t="shared" ca="1" si="23"/>
@@ -4940,14 +4942,14 @@
       <c r="D27" s="19">
         <v>45530</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="24">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="23">
         <v>0.05</v>
       </c>
       <c r="H27" s="15" t="s">
@@ -4961,7 +4963,7 @@
       </c>
       <c r="M27" s="18" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="N27" s="18" t="str">
         <f t="shared" ca="1" si="24"/>
@@ -4977,7 +4979,7 @@
       </c>
       <c r="Q27" s="18" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="R27" s="18" t="str">
         <f t="shared" ca="1" si="24"/>
@@ -5066,14 +5068,14 @@
       <c r="D28" s="19">
         <v>45537</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="24">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="24">
+      <c r="G28" s="23">
         <v>0.05</v>
       </c>
       <c r="H28" s="15" t="s">
@@ -5091,7 +5093,7 @@
       </c>
       <c r="N28" s="18" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="O28" s="18" t="str">
         <f t="shared" ca="1" si="25"/>
@@ -5107,7 +5109,7 @@
       </c>
       <c r="R28" s="18" t="str">
         <f t="shared" ca="1" si="25"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="S28" s="18" t="str">
         <f t="shared" ca="1" si="25"/>
@@ -5192,14 +5194,14 @@
       <c r="D29" s="19">
         <v>45544</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="24">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="23">
         <v>0.05</v>
       </c>
       <c r="H29" s="15" t="s">
@@ -5221,7 +5223,7 @@
       </c>
       <c r="O29" s="18" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="P29" s="18" t="str">
         <f t="shared" ca="1" si="26"/>
@@ -5237,7 +5239,7 @@
       </c>
       <c r="S29" s="18" t="str">
         <f t="shared" ca="1" si="26"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="T29" s="18" t="str">
         <f t="shared" ca="1" si="26"/>
@@ -5310,7 +5312,7 @@
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="19">
         <v>45488</v>
@@ -5318,14 +5320,14 @@
       <c r="D30" s="19">
         <v>45600</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="24">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G30" s="24">
+      <c r="G30" s="23">
         <v>0.05</v>
       </c>
       <c r="H30" s="15" t="s">
@@ -5379,7 +5381,7 @@
       </c>
       <c r="W30" s="18" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="X30" s="18" t="str">
         <f t="shared" ca="1" si="27"/>
@@ -5395,7 +5397,7 @@
       </c>
       <c r="AA30" s="18" t="str">
         <f t="shared" ca="1" si="27"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AB30" s="18" t="str">
         <f t="shared" ca="1" si="27"/>
@@ -5436,7 +5438,7 @@
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="19">
         <v>45488</v>
@@ -5444,14 +5446,14 @@
       <c r="D31" s="19">
         <v>45600</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="24">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G31" s="24">
+      <c r="G31" s="23">
         <v>0.05</v>
       </c>
       <c r="H31" s="15" t="s">
@@ -5505,7 +5507,7 @@
       </c>
       <c r="W31" s="18" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="X31" s="18" t="str">
         <f t="shared" ca="1" si="28"/>
@@ -5521,7 +5523,7 @@
       </c>
       <c r="AA31" s="18" t="str">
         <f t="shared" ca="1" si="28"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AB31" s="18" t="str">
         <f t="shared" ca="1" si="28"/>
@@ -5562,7 +5564,7 @@
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="19">
         <v>45488</v>
@@ -5570,14 +5572,14 @@
       <c r="D32" s="19">
         <v>45600</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="24">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="24">
+      <c r="G32" s="23">
         <v>0.05</v>
       </c>
       <c r="H32" s="15" t="s">
@@ -5631,7 +5633,7 @@
       </c>
       <c r="W32" s="18" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="X32" s="18" t="str">
         <f t="shared" ca="1" si="29"/>
@@ -5647,7 +5649,7 @@
       </c>
       <c r="AA32" s="18" t="str">
         <f t="shared" ca="1" si="29"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AB32" s="18" t="str">
         <f t="shared" ca="1" si="29"/>
@@ -5688,7 +5690,7 @@
     </row>
     <row r="33" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" s="19">
         <v>45600</v>
@@ -5696,14 +5698,14 @@
       <c r="D33" s="19">
         <v>45614</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="24">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G33" s="24">
+      <c r="G33" s="23">
         <v>0.05</v>
       </c>
       <c r="H33" s="15" t="s">
@@ -5765,7 +5767,7 @@
       </c>
       <c r="Y33" s="18" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Z33" s="18" t="str">
         <f t="shared" ca="1" si="30"/>
@@ -5781,7 +5783,7 @@
       </c>
       <c r="AC33" s="18" t="str">
         <f t="shared" ca="1" si="30"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AD33" s="18" t="str">
         <f t="shared" ca="1" si="30"/>
@@ -5814,7 +5816,7 @@
     </row>
     <row r="34" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="19">
         <v>45488</v>
@@ -5822,14 +5824,14 @@
       <c r="D34" s="19">
         <v>45614</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="24">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G34" s="24">
+      <c r="G34" s="23">
         <v>0.05</v>
       </c>
       <c r="H34" s="15" t="s">
@@ -5891,7 +5893,7 @@
       </c>
       <c r="Y34" s="18" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Z34" s="18" t="str">
         <f t="shared" ca="1" si="31"/>
@@ -5907,7 +5909,7 @@
       </c>
       <c r="AC34" s="18" t="str">
         <f t="shared" ca="1" si="31"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AD34" s="18" t="str">
         <f t="shared" ca="1" si="31"/>
@@ -5940,7 +5942,7 @@
     </row>
     <row r="35" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="19">
         <v>45488</v>
@@ -5948,24 +5950,24 @@
       <c r="D35" s="19">
         <v>45495</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="24">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="24">
+      <c r="G35" s="23">
         <v>0.05</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
       <c r="L35" s="18" t="str">
         <f t="shared" ref="L35:AJ35" ca="1" si="32">IF(M$3=($D35-WEEKDAY($D35,2)+1),"u","")</f>
-        <v>u</v>
+        <v/>
       </c>
       <c r="M35" s="18" t="str">
         <f t="shared" ca="1" si="32"/>
@@ -6066,7 +6068,7 @@
     </row>
     <row r="36" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" s="19">
         <v>45488</v>
@@ -6074,24 +6076,24 @@
       <c r="D36" s="19">
         <v>45495</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="24">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G36" s="24">
+      <c r="G36" s="23">
         <v>0.05</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
       <c r="L36" s="18" t="str">
         <f t="shared" ref="L36:AJ36" ca="1" si="33">IF(M$3=($D36-WEEKDAY($D36,2)+1),"u","")</f>
-        <v>u</v>
+        <v/>
       </c>
       <c r="M36" s="18" t="str">
         <f t="shared" ca="1" si="33"/>
@@ -6192,7 +6194,7 @@
     </row>
     <row r="37" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="19">
         <v>45495</v>
@@ -6201,18 +6203,18 @@
         <f t="shared" ref="D37:D45" si="34">C37+7</f>
         <v>45502</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E37" s="24">
         <f t="shared" ref="E37:E68" si="35">IF(D37="","",NETWORKDAYS(C37,D37))</f>
         <v>6</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G37" s="24">
+      <c r="G37" s="23">
         <v>0.05</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
@@ -6222,7 +6224,7 @@
       </c>
       <c r="M37" s="18" t="str">
         <f t="shared" ca="1" si="36"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="N37" s="18" t="str">
         <f t="shared" ca="1" si="36"/>
@@ -6319,7 +6321,7 @@
     </row>
     <row r="38" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" s="19">
         <v>45495</v>
@@ -6328,18 +6330,18 @@
         <f t="shared" si="34"/>
         <v>45502</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G38" s="24">
+      <c r="G38" s="23">
         <v>0.05</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
@@ -6349,7 +6351,7 @@
       </c>
       <c r="M38" s="18" t="str">
         <f t="shared" ca="1" si="37"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="N38" s="18" t="str">
         <f t="shared" ca="1" si="37"/>
@@ -6446,7 +6448,7 @@
     </row>
     <row r="39" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" s="19">
         <f>D37</f>
@@ -6456,18 +6458,18 @@
         <f t="shared" si="34"/>
         <v>45509</v>
       </c>
-      <c r="E39" s="25">
+      <c r="E39" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G39" s="23">
         <v>0.05</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J39" s="17"/>
       <c r="K39" s="17"/>
@@ -6481,7 +6483,7 @@
       </c>
       <c r="N39" s="18" t="str">
         <f t="shared" ca="1" si="38"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="O39" s="18" t="str">
         <f t="shared" ca="1" si="38"/>
@@ -6574,7 +6576,7 @@
     </row>
     <row r="40" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C40" s="19">
         <v>45502</v>
@@ -6583,18 +6585,18 @@
         <f t="shared" si="34"/>
         <v>45509</v>
       </c>
-      <c r="E40" s="25">
+      <c r="E40" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G40" s="24">
+      <c r="G40" s="23">
         <v>0.05</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
@@ -6608,7 +6610,7 @@
       </c>
       <c r="N40" s="18" t="str">
         <f t="shared" ca="1" si="39"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="O40" s="18" t="str">
         <f t="shared" ca="1" si="39"/>
@@ -6701,7 +6703,7 @@
     </row>
     <row r="41" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" s="19">
         <v>45509</v>
@@ -6710,18 +6712,18 @@
         <f t="shared" si="34"/>
         <v>45516</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E41" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="23">
         <v>0.05</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
@@ -6739,7 +6741,7 @@
       </c>
       <c r="O41" s="18" t="str">
         <f t="shared" ca="1" si="40"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="P41" s="18" t="str">
         <f t="shared" ca="1" si="40"/>
@@ -6828,7 +6830,7 @@
     </row>
     <row r="42" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="19">
         <v>45509</v>
@@ -6837,18 +6839,18 @@
         <f t="shared" si="34"/>
         <v>45516</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E42" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G42" s="23">
         <v>0.05</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J42" s="17"/>
       <c r="K42" s="17"/>
@@ -6866,7 +6868,7 @@
       </c>
       <c r="O42" s="18" t="str">
         <f t="shared" ca="1" si="41"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="P42" s="18" t="str">
         <f t="shared" ca="1" si="41"/>
@@ -6955,7 +6957,7 @@
     </row>
     <row r="43" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" s="19">
         <v>45516</v>
@@ -6964,24 +6966,24 @@
         <f t="shared" si="34"/>
         <v>45523</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G43" s="24">
+      <c r="G43" s="23">
         <v>0.05</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J43" s="17"/>
       <c r="K43" s="17"/>
       <c r="L43" s="18" t="str">
         <f t="shared" ref="L43:AJ43" ca="1" si="42">IF(M$3=($D43-WEEKDAY($D43,2)+1),"u","")</f>
-        <v/>
+        <v>u</v>
       </c>
       <c r="M43" s="18" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -6997,7 +6999,7 @@
       </c>
       <c r="P43" s="18" t="str">
         <f t="shared" ca="1" si="42"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="Q43" s="18" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -7082,7 +7084,7 @@
     </row>
     <row r="44" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C44" s="19">
         <v>45516</v>
@@ -7091,24 +7093,24 @@
         <f t="shared" si="34"/>
         <v>45523</v>
       </c>
-      <c r="E44" s="25">
+      <c r="E44" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G44" s="24">
+      <c r="G44" s="23">
         <v>0.05</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J44" s="17"/>
       <c r="K44" s="17"/>
       <c r="L44" s="18" t="str">
         <f t="shared" ref="L44:AJ44" ca="1" si="43">IF(M$3=($D44-WEEKDAY($D44,2)+1),"u","")</f>
-        <v/>
+        <v>u</v>
       </c>
       <c r="M44" s="18" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -7124,7 +7126,7 @@
       </c>
       <c r="P44" s="18" t="str">
         <f t="shared" ca="1" si="43"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="Q44" s="18" t="str">
         <f t="shared" ca="1" si="43"/>
@@ -7209,7 +7211,7 @@
     </row>
     <row r="45" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" s="19">
         <v>45523</v>
@@ -7218,18 +7220,18 @@
         <f t="shared" si="34"/>
         <v>45530</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G45" s="24">
+      <c r="G45" s="23">
         <v>0.05</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J45" s="17"/>
       <c r="K45" s="17"/>
@@ -7239,7 +7241,7 @@
       </c>
       <c r="M45" s="18" t="str">
         <f t="shared" ca="1" si="44"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="N45" s="18" t="str">
         <f t="shared" ca="1" si="44"/>
@@ -7255,7 +7257,7 @@
       </c>
       <c r="Q45" s="18" t="str">
         <f t="shared" ca="1" si="44"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="R45" s="18" t="str">
         <f t="shared" ca="1" si="44"/>
@@ -7335,7 +7337,7 @@
       </c>
     </row>
     <row r="46" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="40" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="19">
@@ -7344,18 +7346,18 @@
       <c r="D46" s="19">
         <v>45530</v>
       </c>
-      <c r="E46" s="25">
+      <c r="E46" s="24">
         <f t="shared" si="35"/>
         <v>11</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G46" s="24">
+      <c r="G46" s="23">
         <v>0.05</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
@@ -7365,7 +7367,7 @@
       </c>
       <c r="M46" s="18" t="str">
         <f t="shared" ca="1" si="45"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="N46" s="18" t="str">
         <f t="shared" ca="1" si="45"/>
@@ -7381,7 +7383,7 @@
       </c>
       <c r="Q46" s="18" t="str">
         <f t="shared" ca="1" si="45"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="R46" s="18" t="str">
         <f t="shared" ca="1" si="45"/>
@@ -7462,7 +7464,7 @@
     </row>
     <row r="47" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="19">
         <v>45523</v>
@@ -7471,18 +7473,18 @@
         <f>C47+7</f>
         <v>45530</v>
       </c>
-      <c r="E47" s="25">
+      <c r="E47" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G47" s="24">
+      <c r="G47" s="23">
         <v>0.05</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J47" s="17"/>
       <c r="K47" s="17"/>
@@ -7492,7 +7494,7 @@
       </c>
       <c r="M47" s="18" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="N47" s="18" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -7508,7 +7510,7 @@
       </c>
       <c r="Q47" s="18" t="str">
         <f t="shared" ca="1" si="46"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="R47" s="18" t="str">
         <f t="shared" ca="1" si="46"/>
@@ -7589,7 +7591,7 @@
     </row>
     <row r="48" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C48" s="19">
         <v>45530</v>
@@ -7598,18 +7600,18 @@
         <f>C48+7</f>
         <v>45537</v>
       </c>
-      <c r="E48" s="25">
+      <c r="E48" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G48" s="24">
+      <c r="G48" s="23">
         <v>0.05</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
@@ -7623,7 +7625,7 @@
       </c>
       <c r="N48" s="18" t="str">
         <f t="shared" ca="1" si="47"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="O48" s="18" t="str">
         <f t="shared" ca="1" si="47"/>
@@ -7639,7 +7641,7 @@
       </c>
       <c r="R48" s="18" t="str">
         <f t="shared" ca="1" si="47"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="S48" s="18" t="str">
         <f t="shared" ca="1" si="47"/>
@@ -7716,7 +7718,7 @@
     </row>
     <row r="49" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C49" s="19">
         <v>45516</v>
@@ -7724,18 +7726,18 @@
       <c r="D49" s="19">
         <v>45537</v>
       </c>
-      <c r="E49" s="25">
+      <c r="E49" s="24">
         <f t="shared" si="35"/>
         <v>16</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G49" s="24">
+      <c r="G49" s="23">
         <v>0.05</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
@@ -7749,7 +7751,7 @@
       </c>
       <c r="N49" s="18" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="O49" s="18" t="str">
         <f t="shared" ca="1" si="48"/>
@@ -7765,7 +7767,7 @@
       </c>
       <c r="R49" s="18" t="str">
         <f t="shared" ca="1" si="48"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="S49" s="18" t="str">
         <f t="shared" ca="1" si="48"/>
@@ -7842,7 +7844,7 @@
     </row>
     <row r="50" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" s="19">
         <v>45530</v>
@@ -7851,18 +7853,18 @@
         <f>C50+7</f>
         <v>45537</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E50" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G50" s="24">
+      <c r="G50" s="23">
         <v>0.05</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
@@ -7876,7 +7878,7 @@
       </c>
       <c r="N50" s="18" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="O50" s="18" t="str">
         <f t="shared" ca="1" si="49"/>
@@ -7892,7 +7894,7 @@
       </c>
       <c r="R50" s="18" t="str">
         <f t="shared" ca="1" si="49"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="S50" s="18" t="str">
         <f t="shared" ca="1" si="49"/>
@@ -7969,7 +7971,7 @@
     </row>
     <row r="51" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C51" s="19">
         <v>45537</v>
@@ -7978,18 +7980,18 @@
         <f>C51+7</f>
         <v>45544</v>
       </c>
-      <c r="E51" s="25">
+      <c r="E51" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G51" s="24">
+      <c r="G51" s="23">
         <v>0.05</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
@@ -8007,7 +8009,7 @@
       </c>
       <c r="O51" s="18" t="str">
         <f t="shared" ca="1" si="50"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="P51" s="18" t="str">
         <f t="shared" ca="1" si="50"/>
@@ -8023,7 +8025,7 @@
       </c>
       <c r="S51" s="18" t="str">
         <f t="shared" ca="1" si="50"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="T51" s="18" t="str">
         <f t="shared" ca="1" si="50"/>
@@ -8096,7 +8098,7 @@
     </row>
     <row r="52" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C52" s="19">
         <v>45537</v>
@@ -8105,18 +8107,18 @@
         <f>C52+7</f>
         <v>45544</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E52" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G52" s="24">
+      <c r="G52" s="23">
         <v>0.05</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J52" s="17"/>
       <c r="K52" s="17"/>
@@ -8134,7 +8136,7 @@
       </c>
       <c r="O52" s="18" t="str">
         <f t="shared" ca="1" si="51"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="P52" s="18" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -8150,7 +8152,7 @@
       </c>
       <c r="S52" s="18" t="str">
         <f t="shared" ca="1" si="51"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="T52" s="18" t="str">
         <f t="shared" ca="1" si="51"/>
@@ -8223,7 +8225,7 @@
     </row>
     <row r="53" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C53" s="19">
         <v>45530</v>
@@ -8231,18 +8233,18 @@
       <c r="D53" s="19">
         <v>45551</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="24">
         <f t="shared" si="35"/>
         <v>16</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G53" s="24">
+      <c r="G53" s="23">
         <v>0.05</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J53" s="17"/>
       <c r="K53" s="17"/>
@@ -8264,7 +8266,7 @@
       </c>
       <c r="P53" s="18" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Q53" s="18" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -8280,7 +8282,7 @@
       </c>
       <c r="T53" s="18" t="str">
         <f t="shared" ca="1" si="52"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="U53" s="18" t="str">
         <f t="shared" ca="1" si="52"/>
@@ -8349,7 +8351,7 @@
     </row>
     <row r="54" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C54" s="19">
         <v>45544</v>
@@ -8358,18 +8360,18 @@
         <f t="shared" ref="D54:D74" si="53">C54+7</f>
         <v>45551</v>
       </c>
-      <c r="E54" s="25">
+      <c r="E54" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G54" s="24">
+      <c r="G54" s="23">
         <v>0.05</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
@@ -8391,7 +8393,7 @@
       </c>
       <c r="P54" s="18" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Q54" s="18" t="str">
         <f t="shared" ca="1" si="54"/>
@@ -8407,7 +8409,7 @@
       </c>
       <c r="T54" s="18" t="str">
         <f t="shared" ca="1" si="54"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="U54" s="18" t="str">
         <f t="shared" ca="1" si="54"/>
@@ -8476,7 +8478,7 @@
     </row>
     <row r="55" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="19">
         <v>45544</v>
@@ -8485,18 +8487,18 @@
         <f t="shared" si="53"/>
         <v>45551</v>
       </c>
-      <c r="E55" s="25">
+      <c r="E55" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G55" s="24">
+      <c r="G55" s="23">
         <v>0.05</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
@@ -8518,7 +8520,7 @@
       </c>
       <c r="P55" s="18" t="str">
         <f t="shared" ca="1" si="55"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Q55" s="18" t="str">
         <f t="shared" ca="1" si="55"/>
@@ -8534,7 +8536,7 @@
       </c>
       <c r="T55" s="18" t="str">
         <f t="shared" ca="1" si="55"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="U55" s="18" t="str">
         <f t="shared" ca="1" si="55"/>
@@ -8603,7 +8605,7 @@
     </row>
     <row r="56" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C56" s="19">
         <v>45551</v>
@@ -8612,18 +8614,18 @@
         <f t="shared" si="53"/>
         <v>45558</v>
       </c>
-      <c r="E56" s="25">
+      <c r="E56" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G56" s="24">
+      <c r="G56" s="23">
         <v>0.05</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J56" s="17"/>
       <c r="K56" s="17"/>
@@ -8649,7 +8651,7 @@
       </c>
       <c r="Q56" s="18" t="str">
         <f t="shared" ca="1" si="56"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="R56" s="18" t="str">
         <f t="shared" ca="1" si="56"/>
@@ -8665,7 +8667,7 @@
       </c>
       <c r="U56" s="18" t="str">
         <f t="shared" ca="1" si="56"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="V56" s="17" t="str">
         <f t="shared" ca="1" si="56"/>
@@ -8730,7 +8732,7 @@
     </row>
     <row r="57" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57" s="19">
         <v>45551</v>
@@ -8739,18 +8741,18 @@
         <f t="shared" si="53"/>
         <v>45558</v>
       </c>
-      <c r="E57" s="25">
+      <c r="E57" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G57" s="24">
+      <c r="G57" s="23">
         <v>0.05</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J57" s="17"/>
       <c r="K57" s="17"/>
@@ -8776,7 +8778,7 @@
       </c>
       <c r="Q57" s="18" t="str">
         <f t="shared" ca="1" si="57"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="R57" s="18" t="str">
         <f t="shared" ca="1" si="57"/>
@@ -8792,7 +8794,7 @@
       </c>
       <c r="U57" s="18" t="str">
         <f t="shared" ca="1" si="57"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="V57" s="17" t="str">
         <f t="shared" ca="1" si="57"/>
@@ -8857,7 +8859,7 @@
     </row>
     <row r="58" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C58" s="19">
         <v>45558</v>
@@ -8866,18 +8868,18 @@
         <f t="shared" si="53"/>
         <v>45565</v>
       </c>
-      <c r="E58" s="25">
+      <c r="E58" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G58" s="24">
+      <c r="G58" s="23">
         <v>0.05</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J58" s="17"/>
       <c r="K58" s="17"/>
@@ -8907,7 +8909,7 @@
       </c>
       <c r="R58" s="18" t="str">
         <f t="shared" ca="1" si="58"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="S58" s="18" t="str">
         <f t="shared" ca="1" si="58"/>
@@ -8923,7 +8925,7 @@
       </c>
       <c r="V58" s="17" t="str">
         <f t="shared" ca="1" si="58"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="W58" s="18" t="str">
         <f t="shared" ca="1" si="58"/>
@@ -8984,7 +8986,7 @@
     </row>
     <row r="59" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C59" s="19">
         <v>45558</v>
@@ -8993,18 +8995,18 @@
         <f t="shared" si="53"/>
         <v>45565</v>
       </c>
-      <c r="E59" s="25">
+      <c r="E59" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G59" s="24">
+      <c r="G59" s="23">
         <v>0.05</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J59" s="17"/>
       <c r="K59" s="17"/>
@@ -9034,7 +9036,7 @@
       </c>
       <c r="R59" s="18" t="str">
         <f t="shared" ca="1" si="59"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="S59" s="18" t="str">
         <f t="shared" ca="1" si="59"/>
@@ -9050,7 +9052,7 @@
       </c>
       <c r="V59" s="17" t="str">
         <f t="shared" ca="1" si="59"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="W59" s="18" t="str">
         <f t="shared" ca="1" si="59"/>
@@ -9111,7 +9113,7 @@
     </row>
     <row r="60" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C60" s="19">
         <v>45565</v>
@@ -9120,18 +9122,18 @@
         <f t="shared" si="53"/>
         <v>45572</v>
       </c>
-      <c r="E60" s="25">
+      <c r="E60" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G60" s="24">
+      <c r="G60" s="23">
         <v>0.05</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J60" s="17"/>
       <c r="K60" s="17"/>
@@ -9165,7 +9167,7 @@
       </c>
       <c r="S60" s="18" t="str">
         <f t="shared" ca="1" si="60"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="T60" s="18" t="str">
         <f t="shared" ca="1" si="60"/>
@@ -9181,7 +9183,7 @@
       </c>
       <c r="W60" s="18" t="str">
         <f t="shared" ca="1" si="60"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="X60" s="18" t="str">
         <f t="shared" ca="1" si="60"/>
@@ -9238,7 +9240,7 @@
     </row>
     <row r="61" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C61" s="19">
         <v>45565</v>
@@ -9247,18 +9249,18 @@
         <f t="shared" si="53"/>
         <v>45572</v>
       </c>
-      <c r="E61" s="25">
+      <c r="E61" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G61" s="24">
+      <c r="G61" s="23">
         <v>0.05</v>
       </c>
       <c r="H61" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J61" s="17"/>
       <c r="K61" s="17"/>
@@ -9292,7 +9294,7 @@
       </c>
       <c r="S61" s="18" t="str">
         <f t="shared" ca="1" si="61"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="T61" s="18" t="str">
         <f t="shared" ca="1" si="61"/>
@@ -9308,7 +9310,7 @@
       </c>
       <c r="W61" s="18" t="str">
         <f t="shared" ca="1" si="61"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="X61" s="18" t="str">
         <f t="shared" ca="1" si="61"/>
@@ -9365,7 +9367,7 @@
     </row>
     <row r="62" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C62" s="19">
         <v>45572</v>
@@ -9374,18 +9376,18 @@
         <f t="shared" si="53"/>
         <v>45579</v>
       </c>
-      <c r="E62" s="25">
+      <c r="E62" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G62" s="24">
+      <c r="G62" s="23">
         <v>0.05</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J62" s="17"/>
       <c r="K62" s="17"/>
@@ -9423,7 +9425,7 @@
       </c>
       <c r="T62" s="18" t="str">
         <f t="shared" ca="1" si="62"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="U62" s="18" t="str">
         <f t="shared" ca="1" si="62"/>
@@ -9439,7 +9441,7 @@
       </c>
       <c r="X62" s="18" t="str">
         <f t="shared" ca="1" si="62"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="Y62" s="18" t="str">
         <f t="shared" ca="1" si="62"/>
@@ -9492,7 +9494,7 @@
     </row>
     <row r="63" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C63" s="19">
         <v>45572</v>
@@ -9501,18 +9503,18 @@
         <f t="shared" si="53"/>
         <v>45579</v>
       </c>
-      <c r="E63" s="25">
+      <c r="E63" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G63" s="24">
+      <c r="G63" s="23">
         <v>0.05</v>
       </c>
       <c r="H63" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J63" s="17"/>
       <c r="K63" s="17"/>
@@ -9550,7 +9552,7 @@
       </c>
       <c r="T63" s="18" t="str">
         <f t="shared" ca="1" si="63"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="U63" s="18" t="str">
         <f t="shared" ca="1" si="63"/>
@@ -9566,7 +9568,7 @@
       </c>
       <c r="X63" s="18" t="str">
         <f t="shared" ca="1" si="63"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="Y63" s="18" t="str">
         <f t="shared" ca="1" si="63"/>
@@ -9619,7 +9621,7 @@
     </row>
     <row r="64" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B64" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C64" s="19">
         <v>45579</v>
@@ -9628,18 +9630,18 @@
         <f t="shared" si="53"/>
         <v>45586</v>
       </c>
-      <c r="E64" s="25">
+      <c r="E64" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G64" s="24">
+      <c r="G64" s="23">
         <v>0.05</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J64" s="17"/>
       <c r="K64" s="17"/>
@@ -9681,7 +9683,7 @@
       </c>
       <c r="U64" s="18" t="str">
         <f t="shared" ca="1" si="64"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="V64" s="17" t="str">
         <f t="shared" ca="1" si="64"/>
@@ -9697,7 +9699,7 @@
       </c>
       <c r="Y64" s="18" t="str">
         <f t="shared" ca="1" si="64"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="Z64" s="18" t="str">
         <f t="shared" ca="1" si="64"/>
@@ -9746,7 +9748,7 @@
     </row>
     <row r="65" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C65" s="19">
         <v>45579</v>
@@ -9755,18 +9757,18 @@
         <f t="shared" si="53"/>
         <v>45586</v>
       </c>
-      <c r="E65" s="25">
+      <c r="E65" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G65" s="24">
+      <c r="G65" s="23">
         <v>0.05</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J65" s="17"/>
       <c r="K65" s="17"/>
@@ -9808,7 +9810,7 @@
       </c>
       <c r="U65" s="18" t="str">
         <f t="shared" ca="1" si="65"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="V65" s="17" t="str">
         <f t="shared" ca="1" si="65"/>
@@ -9824,7 +9826,7 @@
       </c>
       <c r="Y65" s="18" t="str">
         <f t="shared" ca="1" si="65"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="Z65" s="18" t="str">
         <f t="shared" ca="1" si="65"/>
@@ -9873,7 +9875,7 @@
     </row>
     <row r="66" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C66" s="19">
         <v>45586</v>
@@ -9882,18 +9884,18 @@
         <f t="shared" si="53"/>
         <v>45593</v>
       </c>
-      <c r="E66" s="25">
+      <c r="E66" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G66" s="24">
+      <c r="G66" s="23">
         <v>0.05</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J66" s="17"/>
       <c r="K66" s="17"/>
@@ -9939,7 +9941,7 @@
       </c>
       <c r="V66" s="17" t="str">
         <f t="shared" ca="1" si="66"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="W66" s="18" t="str">
         <f t="shared" ca="1" si="66"/>
@@ -9955,7 +9957,7 @@
       </c>
       <c r="Z66" s="18" t="str">
         <f t="shared" ca="1" si="66"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AA66" s="18" t="str">
         <f t="shared" ca="1" si="66"/>
@@ -10000,7 +10002,7 @@
     </row>
     <row r="67" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C67" s="19">
         <v>45586</v>
@@ -10009,18 +10011,18 @@
         <f t="shared" si="53"/>
         <v>45593</v>
       </c>
-      <c r="E67" s="25">
+      <c r="E67" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G67" s="24">
+      <c r="G67" s="23">
         <v>0.05</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J67" s="17"/>
       <c r="K67" s="17"/>
@@ -10066,7 +10068,7 @@
       </c>
       <c r="V67" s="17" t="str">
         <f t="shared" ca="1" si="67"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="W67" s="18" t="str">
         <f t="shared" ca="1" si="67"/>
@@ -10082,7 +10084,7 @@
       </c>
       <c r="Z67" s="18" t="str">
         <f t="shared" ca="1" si="67"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AA67" s="18" t="str">
         <f t="shared" ca="1" si="67"/>
@@ -10127,7 +10129,7 @@
     </row>
     <row r="68" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C68" s="19">
         <v>45593</v>
@@ -10136,18 +10138,18 @@
         <f t="shared" si="53"/>
         <v>45600</v>
       </c>
-      <c r="E68" s="25">
+      <c r="E68" s="24">
         <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G68" s="24">
+      <c r="G68" s="23">
         <v>0.05</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J68" s="17"/>
       <c r="K68" s="17"/>
@@ -10197,7 +10199,7 @@
       </c>
       <c r="W68" s="18" t="str">
         <f t="shared" ca="1" si="68"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="X68" s="18" t="str">
         <f t="shared" ca="1" si="68"/>
@@ -10213,7 +10215,7 @@
       </c>
       <c r="AA68" s="18" t="str">
         <f t="shared" ca="1" si="68"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AB68" s="18" t="str">
         <f t="shared" ca="1" si="68"/>
@@ -10254,7 +10256,7 @@
     </row>
     <row r="69" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C69" s="19">
         <v>45593</v>
@@ -10263,18 +10265,18 @@
         <f t="shared" si="53"/>
         <v>45600</v>
       </c>
-      <c r="E69" s="25">
-        <f t="shared" ref="E69:E100" si="69">IF(D69="","",NETWORKDAYS(C69,D69))</f>
+      <c r="E69" s="24">
+        <f t="shared" ref="E69:E83" si="69">IF(D69="","",NETWORKDAYS(C69,D69))</f>
         <v>6</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G69" s="24">
+      <c r="G69" s="23">
         <v>0.05</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J69" s="17"/>
       <c r="K69" s="17"/>
@@ -10324,7 +10326,7 @@
       </c>
       <c r="W69" s="18" t="str">
         <f t="shared" ca="1" si="70"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="X69" s="18" t="str">
         <f t="shared" ca="1" si="70"/>
@@ -10340,7 +10342,7 @@
       </c>
       <c r="AA69" s="18" t="str">
         <f t="shared" ca="1" si="70"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AB69" s="18" t="str">
         <f t="shared" ca="1" si="70"/>
@@ -10381,7 +10383,7 @@
     </row>
     <row r="70" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C70" s="19">
         <v>45600</v>
@@ -10390,18 +10392,18 @@
         <f t="shared" si="53"/>
         <v>45607</v>
       </c>
-      <c r="E70" s="25">
+      <c r="E70" s="24">
         <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G70" s="24">
+      <c r="G70" s="23">
         <v>0.05</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J70" s="17"/>
       <c r="K70" s="17"/>
@@ -10455,7 +10457,7 @@
       </c>
       <c r="X70" s="18" t="str">
         <f t="shared" ca="1" si="71"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Y70" s="18" t="str">
         <f t="shared" ca="1" si="71"/>
@@ -10471,7 +10473,7 @@
       </c>
       <c r="AB70" s="18" t="str">
         <f t="shared" ca="1" si="71"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AC70" s="18" t="str">
         <f t="shared" ca="1" si="71"/>
@@ -10508,7 +10510,7 @@
     </row>
     <row r="71" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C71" s="19">
         <v>45600</v>
@@ -10517,18 +10519,18 @@
         <f t="shared" si="53"/>
         <v>45607</v>
       </c>
-      <c r="E71" s="25">
+      <c r="E71" s="24">
         <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G71" s="24">
+      <c r="G71" s="23">
         <v>0.05</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J71" s="17"/>
       <c r="K71" s="17"/>
@@ -10582,7 +10584,7 @@
       </c>
       <c r="X71" s="18" t="str">
         <f t="shared" ca="1" si="72"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Y71" s="18" t="str">
         <f t="shared" ca="1" si="72"/>
@@ -10598,7 +10600,7 @@
       </c>
       <c r="AB71" s="18" t="str">
         <f t="shared" ca="1" si="72"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AC71" s="18" t="str">
         <f t="shared" ca="1" si="72"/>
@@ -10635,7 +10637,7 @@
     </row>
     <row r="72" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C72" s="19">
         <v>45607</v>
@@ -10644,18 +10646,18 @@
         <f t="shared" si="53"/>
         <v>45614</v>
       </c>
-      <c r="E72" s="25">
+      <c r="E72" s="24">
         <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G72" s="24">
+      <c r="G72" s="23">
         <v>0.05</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J72" s="17"/>
       <c r="K72" s="17"/>
@@ -10713,7 +10715,7 @@
       </c>
       <c r="Y72" s="18" t="str">
         <f t="shared" ca="1" si="73"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Z72" s="18" t="str">
         <f t="shared" ca="1" si="73"/>
@@ -10729,7 +10731,7 @@
       </c>
       <c r="AC72" s="18" t="str">
         <f t="shared" ca="1" si="73"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AD72" s="18" t="str">
         <f t="shared" ca="1" si="73"/>
@@ -10762,7 +10764,7 @@
     </row>
     <row r="73" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C73" s="19">
         <v>45607</v>
@@ -10771,18 +10773,18 @@
         <f t="shared" si="53"/>
         <v>45614</v>
       </c>
-      <c r="E73" s="25">
+      <c r="E73" s="24">
         <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G73" s="24">
+      <c r="G73" s="23">
         <v>0.05</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J73" s="17"/>
       <c r="K73" s="17"/>
@@ -10840,7 +10842,7 @@
       </c>
       <c r="Y73" s="18" t="str">
         <f t="shared" ca="1" si="74"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Z73" s="18" t="str">
         <f t="shared" ca="1" si="74"/>
@@ -10856,7 +10858,7 @@
       </c>
       <c r="AC73" s="18" t="str">
         <f t="shared" ca="1" si="74"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AD73" s="18" t="str">
         <f t="shared" ca="1" si="74"/>
@@ -10889,7 +10891,7 @@
     </row>
     <row r="74" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C74" s="19">
         <v>45614</v>
@@ -10898,18 +10900,18 @@
         <f t="shared" si="53"/>
         <v>45621</v>
       </c>
-      <c r="E74" s="25">
+      <c r="E74" s="24">
         <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G74" s="24">
+      <c r="G74" s="23">
         <v>0.05</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J74" s="17"/>
       <c r="K74" s="17"/>
@@ -10971,7 +10973,7 @@
       </c>
       <c r="Z74" s="18" t="str">
         <f t="shared" ca="1" si="75"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="AA74" s="18" t="str">
         <f t="shared" ca="1" si="75"/>
@@ -10987,7 +10989,7 @@
       </c>
       <c r="AD74" s="18" t="str">
         <f t="shared" ca="1" si="75"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AE74" s="18" t="str">
         <f t="shared" ca="1" si="75"/>
@@ -11016,7 +11018,7 @@
     </row>
     <row r="75" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C75" s="19">
         <v>45516</v>
@@ -11024,18 +11026,18 @@
       <c r="D75" s="19">
         <v>45621</v>
       </c>
-      <c r="E75" s="25">
+      <c r="E75" s="24">
         <f t="shared" si="69"/>
         <v>76</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G75" s="24">
+      <c r="G75" s="23">
         <v>0.05</v>
       </c>
       <c r="H75" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J75" s="17"/>
       <c r="K75" s="17"/>
@@ -11097,7 +11099,7 @@
       </c>
       <c r="Z75" s="18" t="str">
         <f t="shared" ca="1" si="76"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="AA75" s="18" t="str">
         <f t="shared" ca="1" si="76"/>
@@ -11113,7 +11115,7 @@
       </c>
       <c r="AD75" s="18" t="str">
         <f t="shared" ca="1" si="76"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AE75" s="18" t="str">
         <f t="shared" ca="1" si="76"/>
@@ -11142,7 +11144,7 @@
     </row>
     <row r="76" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C76" s="19">
         <v>45614</v>
@@ -11151,18 +11153,18 @@
         <f>C76+7</f>
         <v>45621</v>
       </c>
-      <c r="E76" s="25">
+      <c r="E76" s="24">
         <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G76" s="24">
+      <c r="G76" s="23">
         <v>0.05</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J76" s="17"/>
       <c r="K76" s="17"/>
@@ -11224,7 +11226,7 @@
       </c>
       <c r="Z76" s="18" t="str">
         <f t="shared" ca="1" si="77"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="AA76" s="18" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -11240,7 +11242,7 @@
       </c>
       <c r="AD76" s="18" t="str">
         <f t="shared" ca="1" si="77"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AE76" s="18" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -11269,7 +11271,7 @@
     </row>
     <row r="77" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C77" s="19">
         <v>45621</v>
@@ -11278,18 +11280,18 @@
         <f>C77+7</f>
         <v>45628</v>
       </c>
-      <c r="E77" s="25">
+      <c r="E77" s="24">
         <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G77" s="24">
+      <c r="G77" s="23">
         <v>0.05</v>
       </c>
       <c r="H77" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J77" s="17"/>
       <c r="K77" s="17"/>
@@ -11355,7 +11357,7 @@
       </c>
       <c r="AA77" s="18" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="AB77" s="18" t="str">
         <f t="shared" ca="1" si="78"/>
@@ -11371,7 +11373,7 @@
       </c>
       <c r="AE77" s="18" t="str">
         <f t="shared" ca="1" si="78"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AF77" s="18" t="str">
         <f t="shared" ca="1" si="78"/>
@@ -11396,7 +11398,7 @@
     </row>
     <row r="78" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C78" s="19">
         <v>45621</v>
@@ -11405,18 +11407,18 @@
         <f>C78+7</f>
         <v>45628</v>
       </c>
-      <c r="E78" s="25">
+      <c r="E78" s="24">
         <f t="shared" si="69"/>
         <v>6</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G78" s="24">
+      <c r="G78" s="23">
         <v>0.05</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J78" s="17"/>
       <c r="K78" s="17"/>
@@ -11482,7 +11484,7 @@
       </c>
       <c r="AA78" s="18" t="str">
         <f t="shared" ca="1" si="79"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="AB78" s="18" t="str">
         <f t="shared" ca="1" si="79"/>
@@ -11498,7 +11500,7 @@
       </c>
       <c r="AE78" s="18" t="str">
         <f t="shared" ca="1" si="79"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="AF78" s="18" t="str">
         <f t="shared" ca="1" si="79"/>
@@ -11522,27 +11524,27 @@
       </c>
     </row>
     <row r="79" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B79" s="22" t="s">
-        <v>29</v>
+      <c r="B79" s="67" t="s">
+        <v>100</v>
       </c>
       <c r="C79" s="19">
-        <v>45488</v>
+        <v>45537</v>
       </c>
       <c r="D79" s="19">
-        <v>45488</v>
-      </c>
-      <c r="E79" s="25">
+        <v>45558</v>
+      </c>
+      <c r="E79" s="24">
         <f t="shared" si="69"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G79" s="24">
+      <c r="G79" s="23">
         <v>0.05</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J79" s="17"/>
       <c r="K79" s="17"/>
@@ -11568,7 +11570,7 @@
       </c>
       <c r="Q79" s="18" t="str">
         <f t="shared" ca="1" si="80"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="R79" s="18" t="str">
         <f t="shared" ca="1" si="80"/>
@@ -11648,16 +11650,28 @@
       </c>
     </row>
     <row r="80" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B80" s="5"/>
-      <c r="C80" s="19"/>
-      <c r="D80" s="19"/>
-      <c r="E80" s="25" t="str">
+      <c r="B80" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C80" s="19">
+        <v>45551</v>
+      </c>
+      <c r="D80" s="19">
+        <v>45607</v>
+      </c>
+      <c r="E80" s="24">
         <f t="shared" si="69"/>
-        <v/>
-      </c>
-      <c r="F80" s="5"/>
-      <c r="G80" s="24"/>
-      <c r="H80" s="15"/>
+        <v>41</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="H80" s="15" t="s">
+        <v>103</v>
+      </c>
       <c r="J80" s="17"/>
       <c r="K80" s="17"/>
       <c r="L80" s="18" t="str">
@@ -11710,7 +11724,7 @@
       </c>
       <c r="X80" s="18" t="str">
         <f t="shared" ca="1" si="81"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="Y80" s="18" t="str">
         <f t="shared" ca="1" si="81"/>
@@ -11762,16 +11776,28 @@
       </c>
     </row>
     <row r="81" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B81" s="5"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="25" t="str">
+      <c r="B81" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C81" s="19">
+        <v>45575</v>
+      </c>
+      <c r="D81" s="19">
+        <v>45635</v>
+      </c>
+      <c r="E81" s="24">
         <f t="shared" si="69"/>
-        <v/>
-      </c>
-      <c r="F81" s="5"/>
-      <c r="G81" s="24"/>
-      <c r="H81" s="15"/>
+        <v>43</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="H81" s="15" t="s">
+        <v>103</v>
+      </c>
       <c r="J81" s="17"/>
       <c r="K81" s="17"/>
       <c r="L81" s="18" t="str">
@@ -11840,7 +11866,7 @@
       </c>
       <c r="AB81" s="18" t="str">
         <f t="shared" ca="1" si="82"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="AC81" s="18" t="str">
         <f t="shared" ca="1" si="82"/>
@@ -11879,12 +11905,12 @@
       <c r="B82" s="5"/>
       <c r="C82" s="19"/>
       <c r="D82" s="19"/>
-      <c r="E82" s="25" t="str">
+      <c r="E82" s="24" t="str">
         <f t="shared" si="69"/>
         <v/>
       </c>
       <c r="F82" s="5"/>
-      <c r="G82" s="24"/>
+      <c r="G82" s="23"/>
       <c r="H82" s="15"/>
       <c r="J82" s="17"/>
       <c r="K82" s="17"/>
@@ -11993,12 +12019,12 @@
       <c r="B83" s="5"/>
       <c r="C83" s="19"/>
       <c r="D83" s="19"/>
-      <c r="E83" s="25" t="str">
+      <c r="E83" s="24" t="str">
         <f t="shared" si="69"/>
         <v/>
       </c>
       <c r="F83" s="5"/>
-      <c r="G83" s="24"/>
+      <c r="G83" s="23"/>
       <c r="H83" s="15"/>
       <c r="J83" s="17"/>
       <c r="K83" s="17"/>
@@ -12104,93 +12130,93 @@
       </c>
     </row>
     <row r="85" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="C85" s="45"/>
-      <c r="D85" s="45"/>
-      <c r="E85" s="46"/>
-      <c r="F85" s="44"/>
-      <c r="G85" s="46"/>
-      <c r="H85" s="47"/>
+      <c r="B85" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="45"/>
+      <c r="F85" s="43"/>
+      <c r="G85" s="45"/>
+      <c r="H85" s="46"/>
     </row>
     <row r="86" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B86" s="49"/>
-      <c r="C86" s="50"/>
-      <c r="D86" s="50"/>
-      <c r="E86" s="51"/>
-      <c r="F86" s="52"/>
-      <c r="G86" s="51"/>
-      <c r="H86" s="53"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="49"/>
+      <c r="E86" s="50"/>
+      <c r="F86" s="51"/>
+      <c r="G86" s="50"/>
+      <c r="H86" s="52"/>
     </row>
     <row r="87" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B87" s="64" t="s">
-        <v>99</v>
-      </c>
-      <c r="C87" s="65" t="s">
-        <v>100</v>
-      </c>
-      <c r="D87" s="55"/>
-      <c r="E87" s="56"/>
-      <c r="F87" s="57"/>
-      <c r="G87" s="56"/>
-      <c r="H87" s="58"/>
+      <c r="B87" s="63" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="D87" s="54"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="56"/>
+      <c r="G87" s="55"/>
+      <c r="H87" s="57"/>
     </row>
     <row r="88" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B88" s="54"/>
-      <c r="C88" s="65" t="s">
-        <v>101</v>
-      </c>
-      <c r="D88" s="55"/>
-      <c r="E88" s="56"/>
-      <c r="F88" s="57"/>
-      <c r="G88" s="56"/>
-      <c r="H88" s="58"/>
+      <c r="B88" s="53"/>
+      <c r="C88" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="D88" s="54"/>
+      <c r="E88" s="55"/>
+      <c r="F88" s="56"/>
+      <c r="G88" s="55"/>
+      <c r="H88" s="57"/>
     </row>
     <row r="89" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B89" s="54"/>
-      <c r="C89" s="55"/>
-      <c r="D89" s="55"/>
-      <c r="E89" s="56"/>
-      <c r="F89" s="57"/>
-      <c r="G89" s="56"/>
-      <c r="H89" s="58"/>
+      <c r="B89" s="53"/>
+      <c r="C89" s="54"/>
+      <c r="D89" s="54"/>
+      <c r="E89" s="55"/>
+      <c r="F89" s="56"/>
+      <c r="G89" s="55"/>
+      <c r="H89" s="57"/>
     </row>
     <row r="90" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B90" s="54"/>
-      <c r="C90" s="55"/>
-      <c r="D90" s="55"/>
-      <c r="E90" s="56"/>
-      <c r="F90" s="57"/>
-      <c r="G90" s="56"/>
-      <c r="H90" s="58"/>
+      <c r="B90" s="53"/>
+      <c r="C90" s="54"/>
+      <c r="D90" s="54"/>
+      <c r="E90" s="55"/>
+      <c r="F90" s="56"/>
+      <c r="G90" s="55"/>
+      <c r="H90" s="57"/>
     </row>
     <row r="91" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B91" s="54"/>
-      <c r="C91" s="55"/>
-      <c r="D91" s="55"/>
-      <c r="E91" s="56"/>
-      <c r="F91" s="57"/>
-      <c r="G91" s="56"/>
-      <c r="H91" s="58"/>
+      <c r="B91" s="53"/>
+      <c r="C91" s="54"/>
+      <c r="D91" s="54"/>
+      <c r="E91" s="55"/>
+      <c r="F91" s="56"/>
+      <c r="G91" s="55"/>
+      <c r="H91" s="57"/>
     </row>
     <row r="92" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B92" s="54"/>
-      <c r="C92" s="55"/>
-      <c r="D92" s="55"/>
-      <c r="E92" s="56"/>
-      <c r="F92" s="57"/>
-      <c r="G92" s="56"/>
-      <c r="H92" s="58"/>
+      <c r="B92" s="53"/>
+      <c r="C92" s="54"/>
+      <c r="D92" s="54"/>
+      <c r="E92" s="55"/>
+      <c r="F92" s="56"/>
+      <c r="G92" s="55"/>
+      <c r="H92" s="57"/>
     </row>
     <row r="93" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="59"/>
-      <c r="C93" s="60"/>
-      <c r="D93" s="60"/>
-      <c r="E93" s="61"/>
-      <c r="F93" s="62"/>
-      <c r="G93" s="61"/>
-      <c r="H93" s="63"/>
+      <c r="B93" s="58"/>
+      <c r="C93" s="59"/>
+      <c r="D93" s="59"/>
+      <c r="E93" s="60"/>
+      <c r="F93" s="61"/>
+      <c r="G93" s="60"/>
+      <c r="H93" s="62"/>
     </row>
   </sheetData>
   <autoFilter ref="B4:H83" xr:uid="{28D10141-A7A4-416F-98C7-DAB7995F3006}">
@@ -12277,7 +12303,7 @@
       <formula>K$3=(TODAY()-WEEKDAY(TODAY(),2)+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H83" xr:uid="{BE294C7B-E1A9-4230-A440-49F41CF44149}">
       <formula1>Subject</formula1>
     </dataValidation>
@@ -12295,7 +12321,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12313,53 +12339,53 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>8</v>
       </c>
       <c r="N2" s="10"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>88</v>
+      <c r="B3" s="30" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
-      <c r="B7" s="37" t="s">
-        <v>89</v>
+      <c r="B7" s="36" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="37" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Misc: Start organising study gantt chart.
</commit_message>
<xml_diff>
--- a/Sem2-Assignments-Gantt-Chart.xlsx
+++ b/Sem2-Assignments-Gantt-Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\TAFE\Dual-Diploma-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB28830-FA5D-4DDD-8EDC-1921A26B5E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC5D5E5-B2C2-4760-A04E-08B1F5188B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A21A907-22B3-4C37-9935-FF093452207E}"/>
   </bookViews>
@@ -1180,13 +1180,13 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1723,10 +1723,10 @@
   <dimension ref="B1:AK93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="9" ySplit="4" topLeftCell="K66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="4" topLeftCell="K52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H79" sqref="H79"/>
+      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,57 +1746,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J1" s="66">
+      <c r="J1" s="67">
         <f ca="1">L3</f>
         <v>45516</v>
       </c>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="65">
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="66">
         <f ca="1">Q3</f>
         <v>45551</v>
       </c>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="66">
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="67">
         <f ca="1">U3</f>
         <v>45579</v>
       </c>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="65">
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="66">
         <f ca="1">Z3</f>
         <v>45614</v>
       </c>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="66">
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="67">
         <f ca="1">AD3</f>
         <v>45642</v>
       </c>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="65">
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="66">
         <f ca="1">AH3</f>
         <v>45670</v>
       </c>
-      <c r="AG1" s="65"/>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="65"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="66"/>
       <c r="AJ1" s="2"/>
     </row>
     <row r="2" spans="2:37" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="22"/>
       <c r="C2" s="42">
         <f ca="1">TODAY()</f>
-        <v>45511</v>
+        <v>45512</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>95</v>
@@ -2727,7 +2727,7 @@
         <v>36</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G10" s="23">
         <v>0.05</v>
@@ -2859,7 +2859,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G11" s="23">
         <v>0.05</v>
@@ -2991,7 +2991,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G12" s="23">
         <v>0.05</v>
@@ -3519,7 +3519,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G16" s="23">
         <v>0.05</v>
@@ -5325,7 +5325,7 @@
         <v>81</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G30" s="23">
         <v>0.05</v>
@@ -5955,7 +5955,7 @@
         <v>6</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G35" s="23">
         <v>0.05</v>
@@ -6081,7 +6081,7 @@
         <v>6</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G36" s="23">
         <v>0.05</v>
@@ -11524,7 +11524,7 @@
       </c>
     </row>
     <row r="79" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B79" s="67" t="s">
+      <c r="B79" s="65" t="s">
         <v>100</v>
       </c>
       <c r="C79" s="19">
@@ -11538,7 +11538,7 @@
         <v>16</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G79" s="23">
         <v>0.05</v>

</xml_diff>